<commit_message>
code is done, testers uploaded as well
</commit_message>
<xml_diff>
--- a/logs csv and results/summary_of_details.xlsx
+++ b/logs csv and results/summary_of_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Desktop\Studies\שנה ב\תכנות מונחה עצמים\Ex0 + 1\logs csv and results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD61C1F0-3861-4D1E-BCF2-AE98222143DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D687DA-86A0-483C-8A56-A3D4D4110AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>amir sabag</t>
   </si>
@@ -33,34 +33,43 @@
     <t>ori darshan</t>
   </si>
   <si>
-    <t>Code Owners,316049311123456789,  Case,9,  Total waiting time: 65372.34007431241,  average waiting time per call: 65.3723400743124,  unCompleted calls,7,  certificate, -316049308979223573</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,8,  Total waiting time: 163617.88209694863,  average waiting time per call: 163.61788209694862,  unCompleted calls,25,  certificate, -316049316554463274</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,7,  Total waiting time: 217606.12115705138,  average waiting time per call: 217.60612115705138,  unCompleted calls,48,  certificate, -316049313375005839</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,6,  Total waiting time: 69162.88209694847,  average waiting time per call: 69.16288209694847,  unCompleted calls,13,  certificate, -316049309085936788</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,5,  Total waiting time: 88035.1211570518,  average waiting time per call: 88.0351211570518,  unCompleted calls,27,  certificate, -316049309710918014</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,4,  Total waiting time: 24783.455368642095,  average waiting time per call: 49.56691073728419,  unCompleted calls,4,  certificate, -316049312692342817</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,3,  Total waiting time: 19117.538284333117,  average waiting time per call: 47.79384571083279,  unCompleted calls,2,  certificate, -316049312627572322</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,2,  Total waiting time: 5095.792822120196,  average waiting time per call: 50.95792822120197,  unCompleted calls,6,  certificate, -316049312658581910</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,1,  Total waiting time: 327.9897426188186,  average waiting time per call: 32.79897426188186,  unCompleted calls,4,  certificate, -316049312106575982</t>
-  </si>
-  <si>
-    <t>Code Owners,316049311123456789,  Case,0,  Total waiting time: 231.9897426188186,  average waiting time per call: 23.19897426188186,  unCompleted calls,0,  certificate, -316049311728397410</t>
+    <t>Code Owners,316049311212458244,  Case,9,  Total waiting time: 62249.34007431242,  average waiting time per call: 62.24934007431242,  unCompleted calls,6,  certificate, -316049312923083330</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,8,  Total waiting time: 139783.88209694857,  average waiting time per call: 139.78388209694856,  unCompleted calls,23,  certificate, -316049315692285783</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,7,  Total waiting time: 177690.12115705168,  average waiting time per call: 177.69012115705166,  unCompleted calls,37,  certificate, -316049316911369233</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,6,  Total waiting time: 66957.88209694847,  average waiting time per call: 66.95788209694847,  unCompleted calls,15,  certificate, -316049308873405043</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,5,  Total waiting time: 78504.1211570518,  average waiting time per call: 78.50412115705181,  unCompleted calls,22,  certificate, -316049309455165983</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,4,  Total waiting time: 23197.455368642088,  average waiting time per call: 46.39491073728418,  unCompleted calls,2,  certificate, -316049312499393040</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,3,  Total waiting time: 19723.538284333124,  average waiting time per call: 49.30884571083281,  unCompleted calls,2,  certificate, -316049312614093487</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,2,  Total waiting time: 5051.792822120196,  average waiting time per call: 50.51792822120196,  unCompleted calls,6,  certificate, -316049312646921093</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,0,  Total waiting time: 231.9897426188186,  average waiting time per call: 23.19897426188186,  unCompleted calls,0,  certificate, -316049311681347185</t>
+  </si>
+  <si>
+    <t>Code Owners,316049311212458244,  Case,1,  Total waiting time: 327.9897426188186,  average waiting time per call: 32.79897426188186,  unCompleted calls,4,  certificate, -316049312126102141</t>
+  </si>
+  <si>
+    <t>מגישים:</t>
+  </si>
+  <si>
+    <t>אמיר סבג</t>
+  </si>
+  <si>
+    <t>אורי דרשן</t>
   </si>
 </sst>
 </file>
@@ -378,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="R3:S17"/>
+  <dimension ref="Q3:S19"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -389,7 +398,7 @@
     <col min="18" max="18" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="18:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="17:19" x14ac:dyDescent="0.25">
       <c r="R3">
         <v>316049311</v>
       </c>
@@ -397,7 +406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="18:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="17:19" x14ac:dyDescent="0.25">
       <c r="R4">
         <v>212458244</v>
       </c>
@@ -405,53 +414,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="18:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8">
+        <v>316049311</v>
+      </c>
       <c r="S8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>212458244</v>
+      </c>
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S10" t="s">
+    <row r="12" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S11" t="s">
+    <row r="13" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S12" t="s">
+    <row r="14" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S13" t="s">
+    <row r="15" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S14" t="s">
+    <row r="16" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="S16" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S19" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>